<commit_message>
add a non-blank in a blank row to verify it isn't a problem (it isn't)
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -406,19 +410,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.625"/>
-    <col min="2" max="2" width="11.875" style="1"/>
-    <col min="4" max="4" width="11.125" style="2"/>
-    <col min="6" max="6" width="13.5"/>
-    <col min="7" max="8" width="20.75"/>
-    <col min="9" max="9" width="38.75"/>
+    <col min="2" max="2" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -468,7 +470,7 @@
         <v>24472.1763888889</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -495,7 +497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -519,12 +521,15 @@
         <v>5844</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -532,5 +537,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>